<commit_message>
Added documents and eagle librarys as well as Part_List.xlsx
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -1,32 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\AMP\Schematic\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F93D29-FCDC-4D53-B4D3-EA811CF992FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D32F4E61-78FC-4918-B891-55F6F71B73CC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -48,7 +32,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -82,16 +66,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -140,7 +121,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -192,7 +173,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -386,23 +367,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C59A17-9116-4A77-A81B-299EAC833C51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added datasheet for dual channel N MOS BSD223P. Added several parts to the Part_list
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\AMP\Schematic\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD03092-B165-4554-9620-25EE5D481E0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>https://de.farnell.com/on-semiconductor/mc78m12cdtrkg/linearer-spann-regler-12v-0-5a/dp/2822588RL</t>
   </si>
@@ -27,16 +32,83 @@
   </si>
   <si>
     <t>Reihenklemme x3</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>Schematic Bezeichner</t>
+  </si>
+  <si>
+    <t>Mouser Link</t>
+  </si>
+  <si>
+    <t>Q5A, Q5B</t>
+  </si>
+  <si>
+    <t>SJ1-3523N</t>
+  </si>
+  <si>
+    <t>BSD223PH6327XTSA1</t>
+  </si>
+  <si>
+    <t>Audio Buchse</t>
+  </si>
+  <si>
+    <t>09HCP-470M-50</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Tiefpass Spule 47uH</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Tiefpass Kapazität</t>
+  </si>
+  <si>
+    <t>smd-kondensator-2220-330nf-100v</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>BSD235NH6327XT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inverter P MOS Pair nach Optokoppler </t>
+  </si>
+  <si>
+    <t>Optokoppler Driver N MOS Pair</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,13 +131,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -73,6 +149,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -367,43 +446,117 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="96.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{CEBACEB6-6688-4F75-B941-D79738B5A125}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{451E794E-B0C6-408F-932F-307F839C59DD}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{E52E1F6D-1D26-4DDD-B0EE-BB034088D669}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{32C8A10D-5B10-439C-80D8-128576016A37}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{5A4B64D3-9F6A-47E6-BDD9-B7E25E35D8CE}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{F04B1ACF-D099-406F-A235-2D3FA0B02A61}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{2C27DC6F-DF29-41B3-81E3-C24904DE5997}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add optocoupler to part list
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD03092-B165-4554-9620-25EE5D481E0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8ED3D6-A6C6-4869-8AA3-FF0054AB2212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>https://de.farnell.com/on-semiconductor/mc78m12cdtrkg/linearer-spann-regler-12v-0-5a/dp/2822588RL</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>Optokoppler Driver N MOS Pair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optokoppler </t>
+  </si>
+  <si>
+    <t>ACPL-064L-000E</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +552,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{CEBACEB6-6688-4F75-B941-D79738B5A125}"/>
@@ -555,8 +569,9 @@
     <hyperlink ref="C5" r:id="rId5" xr:uid="{5A4B64D3-9F6A-47E6-BDD9-B7E25E35D8CE}"/>
     <hyperlink ref="C8" r:id="rId6" xr:uid="{F04B1ACF-D099-406F-A235-2D3FA0B02A61}"/>
     <hyperlink ref="C9" r:id="rId7" xr:uid="{2C27DC6F-DF29-41B3-81E3-C24904DE5997}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{058CFE8C-85EA-4CAC-BEF3-55983CA07CB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adapted wireing width of power stage and exchanged bootstrap capacitor
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\AMP\Schematic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8ED3D6-A6C6-4869-8AA3-FF0054AB2212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F586A27-F891-4825-B1BD-BA859A2548F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>https://de.farnell.com/on-semiconductor/mc78m12cdtrkg/linearer-spann-regler-12v-0-5a/dp/2822588RL</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>ACPL-064L-000E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/TDK/CGA4J1X7R1H475K125AE?qs=PqoDHHvF64%252BKyTaX2qYTwQ%3D%3D </t>
+  </si>
+  <si>
+    <t>C bootstrap</t>
+  </si>
+  <si>
+    <t>C1</t>
   </si>
 </sst>
 </file>
@@ -147,8 +156,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,13 +469,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C10"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
@@ -558,6 +567,17 @@
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -570,8 +590,9 @@
     <hyperlink ref="C8" r:id="rId6" xr:uid="{F04B1ACF-D099-406F-A235-2D3FA0B02A61}"/>
     <hyperlink ref="C9" r:id="rId7" xr:uid="{2C27DC6F-DF29-41B3-81E3-C24904DE5997}"/>
     <hyperlink ref="C10" r:id="rId8" xr:uid="{058CFE8C-85EA-4CAC-BEF3-55983CA07CB6}"/>
+    <hyperlink ref="C11" r:id="rId9" xr:uid="{98B250C1-6D1B-407B-8A34-EFE0AA3D1CD5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ERC and DRC done. Ready for production.
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F586A27-F891-4825-B1BD-BA859A2548F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AE88D4-C36F-4311-A923-987972440F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -267,7 +267,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -472,7 +472,7 @@
   <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add mouser link to fuse
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\AMP\Schematic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AE88D4-C36F-4311-A923-987972440F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19D57F2-3B7D-4118-AF78-EFED6E581421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>https://de.farnell.com/on-semiconductor/mc78m12cdtrkg/linearer-spann-regler-12v-0-5a/dp/2822588RL</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>C1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Bel-Fuse/C1T5?qs=GtFly9OVs8%2FF1GxRAaUoTA%3D%3D</t>
+  </si>
+  <si>
+    <t>Fuse</t>
+  </si>
+  <si>
+    <t>F1-3</t>
   </si>
 </sst>
 </file>
@@ -156,8 +165,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -173,7 +182,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,13 +478,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
@@ -578,6 +587,17 @@
       </c>
       <c r="C11" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -591,8 +611,9 @@
     <hyperlink ref="C9" r:id="rId7" xr:uid="{2C27DC6F-DF29-41B3-81E3-C24904DE5997}"/>
     <hyperlink ref="C10" r:id="rId8" xr:uid="{058CFE8C-85EA-4CAC-BEF3-55983CA07CB6}"/>
     <hyperlink ref="C11" r:id="rId9" xr:uid="{98B250C1-6D1B-407B-8A34-EFE0AA3D1CD5}"/>
+    <hyperlink ref="C12" r:id="rId10" xr:uid="{46392008-F199-4318-9B28-4AE1C8ADBDE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add 3.3V regulator to part list
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19D57F2-3B7D-4118-AF78-EFED6E581421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD406A4-C2B5-4C75-94E6-F79AAFD3092C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5325" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>https://de.farnell.com/on-semiconductor/mc78m12cdtrkg/linearer-spann-regler-12v-0-5a/dp/2822588RL</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>F1-3</t>
+  </si>
+  <si>
+    <t>3.3V Spannungsregler</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/Texas-Instruments/UA78M33CDCY?qs=sbcp%2F4gpy09US8tH%252B2FxOw%3D%3D</t>
+  </si>
+  <si>
+    <t>IC3</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,6 +609,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{CEBACEB6-6688-4F75-B941-D79738B5A125}"/>
@@ -612,8 +632,9 @@
     <hyperlink ref="C10" r:id="rId8" xr:uid="{058CFE8C-85EA-4CAC-BEF3-55983CA07CB6}"/>
     <hyperlink ref="C11" r:id="rId9" xr:uid="{98B250C1-6D1B-407B-8A34-EFE0AA3D1CD5}"/>
     <hyperlink ref="C12" r:id="rId10" xr:uid="{46392008-F199-4318-9B28-4AE1C8ADBDE6}"/>
+    <hyperlink ref="C13" r:id="rId11" xr:uid="{4FACC8D9-F2B2-4867-BFDB-0E1A695BC737}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added parts to part list
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AE88D4-C36F-4311-A923-987972440F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47172F9-0FDD-479C-A945-F3AD9E2FF1BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,21 +16,16 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
-  <si>
-    <t>https://de.farnell.com/on-semiconductor/mc78m12cdtrkg/linearer-spann-regler-12v-0-5a/dp/2822588RL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>12V Spannungsregler</t>
   </si>
   <si>
-    <t>https://de.farnell.com/camdenboss/ctb0305-3/anschlussblock-3polig/dp/3882640</t>
-  </si>
-  <si>
     <t>Reihenklemme x3</t>
   </si>
   <si>
@@ -98,6 +93,117 @@
   </si>
   <si>
     <t>C1</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/ON-Semiconductor/MC78M12CDTG?qs=%252B9%2Fcbd0IE0R3GzHVzfSzCw%3D%3D</t>
+  </si>
+  <si>
+    <t>Reihenklemme x6</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/?qs=qPbxTIUfeZanCGLWbKOtjg%3D%3D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Phoenix-Contact/1984659?qs=FQYO1eEgUPBU2UOuKgfwDQ%3D%3D </t>
+  </si>
+  <si>
+    <t>U$4</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/ROHM-Semiconductor/ESR03EZPJ100?qs=sGAEpiMZZMvdGkrng054t4QdAY%2FQ0Lwevf6%2Fn4jOics%3D </t>
+  </si>
+  <si>
+    <t>Anzahl</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>10 ohm wiederstand</t>
+  </si>
+  <si>
+    <t>R5, 6, 7, 8, 15, 16</t>
+  </si>
+  <si>
+    <t>R3, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/ROHM-Semiconductor/ESR03EZPJ361?qs=sGAEpiMZZMvdGkrng054tywGjayRHxH2OmqZkBvdXCdQDNCcqKyq%252Bw%3D%3D </t>
+  </si>
+  <si>
+    <t>360 ohm wiederstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/ROHM-Semiconductor/ESR03EZPJ102?qs=sGAEpiMZZMvdGkrng054t67Efho1F8r6QhotjvmT7pg%3D </t>
+  </si>
+  <si>
+    <t>1 kohm wiederstand</t>
+  </si>
+  <si>
+    <t>R1, 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/ROHM-Semiconductor/ESR03EZPJ103?qs=sGAEpiMZZMvdGkrng054t67Efho1F8r6e9okZoMz64k%3D </t>
+  </si>
+  <si>
+    <t>10 kohm wiederstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/ROHM-Semiconductor/ESR03EZPJ203?qs=sGAEpiMZZMvdGkrng054tywGjayRHxH2kB02wLOq7F%2Fb6T5685OEtg%3D%3D </t>
+  </si>
+  <si>
+    <t>20 kohm wiederstand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/ROHM-Semiconductor/ESR03EZPJ303?qs=sGAEpiMZZMvdGkrng054tywGjayRHxH24PoxxsN5Rqjy1SoRVZCW9g%3D%3D </t>
+  </si>
+  <si>
+    <t>30 kohm wiederstand</t>
+  </si>
+  <si>
+    <t>C11, C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/KEMET/C0603C104J3REC7411?qs=sGAEpiMZZMuMW9TJLBQkXgnPr%252BLGMrWvu0%2FSw%2FlXXGU%3D </t>
+  </si>
+  <si>
+    <t>100 nF Kondensator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Taiyo-Yuden/TMK107BJ334KA-T?qs=sGAEpiMZZMuMW9TJLBQkXvrk1hHKP5vXULPTKZOflZw%3D </t>
+  </si>
+  <si>
+    <t>330 nF Kondensator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/KEMET/C0603C105Z3VACTU?qs=sGAEpiMZZMuMW9TJLBQkXtQELi8n00gZe2LtScZlwS8%3D </t>
+  </si>
+  <si>
+    <t>1 µF Kondensator</t>
+  </si>
+  <si>
+    <t>C18, C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17, C15, C12, C8, C7, C4, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Vishay-General-Semiconductor/SS1H10-M3-61T?qs=ROh%252BA47s9d2Nfc8fXnSHeQ%3D%3D </t>
+  </si>
+  <si>
+    <t>Freilaufdiode</t>
+  </si>
+  <si>
+    <t>D2, D3</t>
   </si>
 </sst>
 </file>
@@ -469,130 +575,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C11"/>
+  <dimension ref="A2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="151.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{CEBACEB6-6688-4F75-B941-D79738B5A125}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{451E794E-B0C6-408F-932F-307F839C59DD}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{E52E1F6D-1D26-4DDD-B0EE-BB034088D669}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{32C8A10D-5B10-439C-80D8-128576016A37}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{5A4B64D3-9F6A-47E6-BDD9-B7E25E35D8CE}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{F04B1ACF-D099-406F-A235-2D3FA0B02A61}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{2C27DC6F-DF29-41B3-81E3-C24904DE5997}"/>
-    <hyperlink ref="C10" r:id="rId8" xr:uid="{058CFE8C-85EA-4CAC-BEF3-55983CA07CB6}"/>
-    <hyperlink ref="C11" r:id="rId9" xr:uid="{98B250C1-6D1B-407B-8A34-EFE0AA3D1CD5}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{451E794E-B0C6-408F-932F-307F839C59DD}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{E52E1F6D-1D26-4DDD-B0EE-BB034088D669}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{32C8A10D-5B10-439C-80D8-128576016A37}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{5A4B64D3-9F6A-47E6-BDD9-B7E25E35D8CE}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{F04B1ACF-D099-406F-A235-2D3FA0B02A61}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{2C27DC6F-DF29-41B3-81E3-C24904DE5997}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{058CFE8C-85EA-4CAC-BEF3-55983CA07CB6}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{98B250C1-6D1B-407B-8A34-EFE0AA3D1CD5}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{A0CD2489-7DA8-46E2-AE4E-65CFD4FF82F1}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{78672D3A-8053-43BA-AF30-00E1C0334030}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{CD8F65C7-69F9-4E80-963E-BB8B11A9FD82}"/>
+    <hyperlink ref="C16" r:id="rId12" xr:uid="{57975132-4AAF-4A51-8BDE-5A0D81D3B4F8}"/>
+    <hyperlink ref="C17" r:id="rId13" xr:uid="{04E38CCF-D46E-4235-B138-D0A93561FF19}"/>
+    <hyperlink ref="C18" r:id="rId14" xr:uid="{25EB52DB-C2EB-4595-9CD9-9EC2F25E5E28}"/>
+    <hyperlink ref="C19" r:id="rId15" xr:uid="{4782CC45-99D4-44F2-A8E7-364C6D1FC7F0}"/>
+    <hyperlink ref="C20" r:id="rId16" xr:uid="{25EA4E21-15E5-4C48-95AD-BCF09C2DD625}"/>
+    <hyperlink ref="C21" r:id="rId17" xr:uid="{09F6531F-394F-499A-A845-ABDC81E95352}"/>
+    <hyperlink ref="C22" r:id="rId18" xr:uid="{F5306261-264F-484F-ADBA-9FCCDB697181}"/>
+    <hyperlink ref="C23" r:id="rId19" xr:uid="{2BBD1636-D1CB-46C0-AC8A-3CC3CD12979C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dummy change to check connectivity to repository
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erwin\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF1737A-0456-4DC0-88BD-7FC128075ABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB428F2B-8755-4E23-96D6-2A90A861A641}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>12V Spannungsregler</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.mouser.de/ProductDetail/Phoenix-Contact/1984659?qs=FQYO1eEgUPBU2UOuKgfwDQ%3D%3D  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hallo </t>
+  </si>
+  <si>
+    <t>Erwin</t>
   </si>
 </sst>
 </file>
@@ -281,8 +287,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -298,7 +304,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -594,13 +600,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
@@ -906,6 +912,14 @@
       </c>
       <c r="D24">
         <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added non inverting optocoupler as suppliment of ACPL-064L
</commit_message>
<xml_diff>
--- a/Schematic/Part_List.xlsx
+++ b/Schematic/Part_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erwin\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\AMP\Schematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF1737A-0456-4DC0-88BD-7FC128075ABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2FC266-9FE3-4C0E-9537-7E6923253135}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>12V Spannungsregler</t>
   </si>
@@ -70,9 +70,6 @@
     <t>C5</t>
   </si>
   <si>
-    <t>BSD235NH6327XT</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inverter P MOS Pair nach Optokoppler </t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t xml:space="preserve">Optokoppler </t>
   </si>
   <si>
-    <t>ACPL-064L-000E</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.mouser.de/ProductDetail/TDK/CGA4J1X7R1H475K125AE?qs=PqoDHHvF64%252BKyTaX2qYTwQ%3D%3D </t>
   </si>
   <si>
@@ -205,9 +199,6 @@
     <t>Fuse</t>
   </si>
   <si>
-    <t>https://www.mouser.de/ProductDetail/Bel-Fuse/C1T5?qs=GtFly9OVs8%2FF1GxRAaUoTA%3D%3D</t>
-  </si>
-  <si>
     <t>IC3</t>
   </si>
   <si>
@@ -221,6 +212,42 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.mouser.de/ProductDetail/Phoenix-Contact/1984659?qs=FQYO1eEgUPBU2UOuKgfwDQ%3D%3D  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Bourns/SF-1206F500-2?qs=GIQXYiEeHGBJCxGonQTRiw%3D%3D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Texas-Instruments/TMP235AEDBZRQ1?qs=T3oQrply3y9acrBXtVPwnw%3D%3D </t>
+  </si>
+  <si>
+    <t>Temperatursensor</t>
+  </si>
+  <si>
+    <t>IC1, IC4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/TDK/MMZ0603S102HT000?qs=%2Fha2pyFaduhzz9aGpAASO8pUA5u3Z3KfzMOcSgnHg9rOh%2FMvhoxK4g%3D%3D </t>
+  </si>
+  <si>
+    <t>Ferrit bead</t>
+  </si>
+  <si>
+    <t>BEAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Infineon-Technologies/BSD235NH6327XT?qs=zO0nedAqnNLj5BYSlH7kJg%3D%3D </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.de/ProductDetail/?qs=W3wJikR1%252BS6eKzfFl8Rbew%3D%3D </t>
+  </si>
+  <si>
+    <t>Reihenklemme x2</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>https://www.mouser.de/ProductDetail/757-TLP2270TP4E</t>
   </si>
 </sst>
 </file>
@@ -273,12 +300,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -594,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,18 +644,18 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>65</v>
+      <c r="C2" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -637,13 +663,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -654,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -701,13 +727,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -715,13 +741,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -729,52 +755,63 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D13">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -787,17 +824,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,67 +848,73 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D21">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -891,30 +928,74 @@
         <v>61</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" xr:uid="{BED07DA7-0F37-4F7D-83F8-75F79917D748}"/>
+    <hyperlink ref="C23" r:id="rId1" xr:uid="{BED07DA7-0F37-4F7D-83F8-75F79917D748}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{CE971A56-7D88-4150-A11F-E08B33EB2543}"/>
-    <hyperlink ref="C12" r:id="rId3" xr:uid="{5AA02692-7EB3-42F7-96D3-13E7C03B0A29}"/>
+    <hyperlink ref="C11" r:id="rId3" xr:uid="{5AA02692-7EB3-42F7-96D3-13E7C03B0A29}"/>
+    <hyperlink ref="C22" r:id="rId4" xr:uid="{83D8141B-DB9A-45BC-8712-7C7B2C7FB542}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{F1798248-1811-4110-9BB3-EA139C2D3473}"/>
+    <hyperlink ref="C18" r:id="rId6" xr:uid="{89892244-7518-4951-A3A9-BD3500B46A8D}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{5ED9294F-1E91-4957-A54D-C856A51767B3}"/>
+    <hyperlink ref="C24" r:id="rId8" xr:uid="{007241B6-DA99-4F82-8ACC-5C52AADDFE93}"/>
+    <hyperlink ref="C25" r:id="rId9" xr:uid="{E9DC41ED-F1B7-4493-B00E-36B6768B0DBB}"/>
+    <hyperlink ref="C20" r:id="rId10" xr:uid="{4971301B-2905-4C8A-8077-F3D428DC0653}"/>
+    <hyperlink ref="C14" r:id="rId11" xr:uid="{924C3689-81E4-445A-81BB-ACB75E5741AE}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{58400F2D-54BF-4AA9-A68F-23533069A489}"/>
+    <hyperlink ref="C17" r:id="rId13" xr:uid="{9071E884-1A87-42A1-91AA-CC6AD5CD4380}"/>
+    <hyperlink ref="C8" r:id="rId14" xr:uid="{A6A96F09-9D2D-4040-8F3D-85F79EC832B9}"/>
+    <hyperlink ref="C13" r:id="rId15" xr:uid="{1D02B57C-F403-4489-84D5-365C286D5369}"/>
+    <hyperlink ref="C10" r:id="rId16" xr:uid="{A18F59A2-E39F-4C8F-AE83-8E2155BD2ED8}"/>
+    <hyperlink ref="C21" r:id="rId17" xr:uid="{7EE63B0C-53B5-4533-A195-70113C59454A}"/>
+    <hyperlink ref="C26" r:id="rId18" xr:uid="{67B0507B-8177-442E-9725-147DC1C8E8CB}"/>
+    <hyperlink ref="C9" r:id="rId19" xr:uid="{DB0285BA-2975-4E89-88C6-98EA8159F1A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>